<commit_message>
error in plot fixed
</commit_message>
<xml_diff>
--- a/output/Table1.xlsx
+++ b/output/Table1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmatth\Dropbox\Reinfections_and_cross_protection_1918_influenza\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6221BF1B-53BC-4817-A453-600E3EC68C25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAF5163-B22D-412D-A75D-C48E62279FC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17325" xr2:uid="{32B1BB74-3AD3-4DE3-AB21-5204A2169F34}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17328" xr2:uid="{32B1BB74-3AD3-4DE3-AB21-5204A2169F34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -607,16 +607,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515CBF80-7F84-4DA6-B646-0E5E206E836B}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q52" sqref="Q52"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="57" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="16" t="s">
         <v>0</v>
@@ -633,7 +633,7 @@
       </c>
       <c r="I1" s="16"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -656,7 +656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -675,7 +675,7 @@
       </c>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -686,7 +686,7 @@
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -699,7 +699,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>27</v>
       </c>
@@ -718,7 +718,7 @@
       </c>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>35</v>
       </c>
@@ -737,7 +737,7 @@
       </c>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>28</v>
       </c>
@@ -756,7 +756,7 @@
       </c>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
@@ -781,7 +781,7 @@
         <v>41.2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
@@ -806,7 +806,7 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -817,7 +817,7 @@
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -830,7 +830,7 @@
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
@@ -855,7 +855,7 @@
         <v>50.2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>10</v>
       </c>
@@ -880,7 +880,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>7</v>
       </c>
@@ -905,7 +905,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -916,7 +916,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -929,7 +929,7 @@
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>12</v>
       </c>
@@ -954,7 +954,7 @@
         <v>57.8</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>13</v>
       </c>
@@ -979,7 +979,7 @@
         <v>41.3</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>14</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>9</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1040,7 +1040,7 @@
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
@@ -1053,7 +1053,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>9</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>10</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>7</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1139,7 +1139,7 @@
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
@@ -1152,7 +1152,7 @@
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>17</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>79.400000000000006</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>18</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>34</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -1238,7 +1238,7 @@
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -1274,7 +1274,7 @@
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>20</v>
       </c>
@@ -1287,7 +1287,7 @@
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>9</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -1325,7 +1325,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>9</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>45.5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>22</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>23</v>
       </c>
@@ -1413,7 +1413,7 @@
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>9</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>46.3</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>7</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>22</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>24</v>
       </c>
@@ -1501,7 +1501,7 @@
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>9</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>7</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
         <v>22</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>31.8</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>25</v>
       </c>

</xml_diff>